<commit_message>
tutor add class and check
</commit_message>
<xml_diff>
--- a/TestDataXls/tutor_add_class.xlsx
+++ b/TestDataXls/tutor_add_class.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02233390-22E8-43A0-98F8-739BE7FB37CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F370D7-3CFF-4FDE-90F0-FE427576403B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="179">
   <si>
     <t>password</t>
   </si>
@@ -248,9 +248,6 @@
     <t>https://support.zoom.us/hc/en-us/articles/201362843-What-is-Personal-Meeting-ID-PMI-and-Personal-Link-</t>
   </si>
   <si>
-    <t>D:\nurtem\Picturesprofile\mirudhangam.jpg</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -350,9 +347,6 @@
     <t>Every week</t>
   </si>
   <si>
-    <t>D:\test\picturesprofile1\bharat3.jpg</t>
-  </si>
-  <si>
     <t>Test@1234</t>
   </si>
   <si>
@@ -542,16 +536,31 @@
     <t>var class special 29/11 - 31/12</t>
   </si>
   <si>
-    <t>D:\test\picturesprofile1\bharat1.jpg</t>
-  </si>
-  <si>
     <t>paint var 20</t>
   </si>
   <si>
-    <t>01/12/2022</t>
-  </si>
-  <si>
     <t>var class special 01/12 - 31/12</t>
+  </si>
+  <si>
+    <t>D:\nurtem\test\picturesprofile1\bharat3.jpg</t>
+  </si>
+  <si>
+    <t>07/12/2022</t>
+  </si>
+  <si>
+    <t>next_session</t>
+  </si>
+  <si>
+    <t>Wednesday | 7:00 pm to 8:00 pm</t>
+  </si>
+  <si>
+    <t>tutor_name</t>
+  </si>
+  <si>
+    <t>Jaya S.</t>
+  </si>
+  <si>
+    <t>Class_type</t>
   </si>
 </sst>
 </file>
@@ -962,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF39"/>
+  <dimension ref="A1:AJ39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1003,7 +1012,7 @@
     <col min="32" max="32" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1032,7 +1041,7 @@
         <v>19</v>
       </c>
       <c r="J1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -1083,13 +1092,13 @@
         <v>72</v>
       </c>
       <c r="AA1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB1" t="s">
         <v>95</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>96</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>97</v>
       </c>
       <c r="AD1" t="s">
         <v>3</v>
@@ -1100,22 +1109,31 @@
       <c r="AF1" t="s">
         <v>5</v>
       </c>
+      <c r="AG1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>178</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F2" s="8">
         <v>2</v>
@@ -1124,13 +1142,13 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K2" t="s">
         <v>25</v>
@@ -1139,28 +1157,28 @@
         <v>20</v>
       </c>
       <c r="M2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P2">
         <v>1</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R2">
         <v>12</v>
       </c>
       <c r="S2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1172,63 +1190,63 @@
         <v>38</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD2" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE2">
         <v>10</v>
       </c>
       <c r="AF2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" t="s">
         <v>79</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>103</v>
-      </c>
-      <c r="I3" t="s">
-        <v>106</v>
-      </c>
-      <c r="J3" t="s">
-        <v>80</v>
       </c>
       <c r="K3" t="s">
         <v>25</v>
@@ -1237,28 +1255,28 @@
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P3">
         <v>1</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R3">
         <v>12</v>
       </c>
       <c r="S3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1267,66 +1285,66 @@
         <v>39</v>
       </c>
       <c r="W3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB3" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC3" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AE3">
         <v>10</v>
       </c>
       <c r="AF3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>118</v>
+      </c>
+      <c r="I4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" t="s">
         <v>79</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I4" t="s">
-        <v>121</v>
-      </c>
-      <c r="J4" t="s">
-        <v>80</v>
       </c>
       <c r="K4" t="s">
         <v>25</v>
@@ -1335,28 +1353,28 @@
         <v>20</v>
       </c>
       <c r="M4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P4">
         <v>1</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R4">
         <v>12</v>
       </c>
       <c r="S4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -1368,63 +1386,63 @@
         <v>38</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z4" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AB4" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC4" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD4" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE4">
         <v>4</v>
       </c>
       <c r="AF4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E5" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
         <v>109</v>
       </c>
-      <c r="F5" s="8">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>111</v>
-      </c>
       <c r="I5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K5" t="s">
         <v>25</v>
@@ -1433,28 +1451,28 @@
         <v>10</v>
       </c>
       <c r="M5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P5">
         <v>1</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R5">
         <v>12</v>
       </c>
       <c r="S5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -1466,63 +1484,63 @@
         <v>38</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z5" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AB5" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC5" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD5" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE5">
         <v>4</v>
       </c>
       <c r="AF5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>118</v>
+      </c>
+      <c r="I6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" t="s">
         <v>79</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I6" t="s">
-        <v>123</v>
-      </c>
-      <c r="J6" t="s">
-        <v>80</v>
       </c>
       <c r="K6" t="s">
         <v>25</v>
@@ -1531,28 +1549,28 @@
         <v>10</v>
       </c>
       <c r="M6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P6">
         <v>1</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R6">
         <v>12</v>
       </c>
       <c r="S6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -1564,39 +1582,39 @@
         <v>38</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AB6" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC6" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD6" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE6">
         <v>4</v>
       </c>
       <c r="AF6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>27</v>
@@ -1629,22 +1647,22 @@
         <v>24</v>
       </c>
       <c r="N7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R7">
         <v>12</v>
       </c>
       <c r="S7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T7" t="s">
         <v>70</v>
@@ -1659,63 +1677,63 @@
         <v>40</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AB7" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC7" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD7" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE7">
         <v>4</v>
       </c>
       <c r="AF7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" t="s">
         <v>125</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>126</v>
-      </c>
-      <c r="I8" t="s">
-        <v>127</v>
-      </c>
-      <c r="J8" t="s">
-        <v>128</v>
       </c>
       <c r="K8" t="s">
         <v>25</v>
@@ -1727,25 +1745,25 @@
         <v>24</v>
       </c>
       <c r="N8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R8">
         <v>12</v>
       </c>
       <c r="S8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U8">
         <v>60</v>
@@ -1757,22 +1775,22 @@
         <v>41</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z8" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AB8" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC8" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD8" t="s">
         <v>172</v>
@@ -1781,24 +1799,24 @@
         <v>4</v>
       </c>
       <c r="AF8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="3">
         <v>0</v>
@@ -1807,13 +1825,13 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
+        <v>124</v>
+      </c>
+      <c r="I9" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" t="s">
         <v>126</v>
-      </c>
-      <c r="I9" t="s">
-        <v>133</v>
-      </c>
-      <c r="J9" t="s">
-        <v>128</v>
       </c>
       <c r="K9" t="s">
         <v>25</v>
@@ -1825,25 +1843,25 @@
         <v>24</v>
       </c>
       <c r="N9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P9">
         <v>1</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R9">
         <v>12</v>
       </c>
       <c r="S9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U9">
         <v>60</v>
@@ -1855,48 +1873,48 @@
         <v>41</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z9" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA9" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AB9" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC9" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD9" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE9">
         <v>4</v>
       </c>
       <c r="AF9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="3">
         <v>0</v>
@@ -1905,13 +1923,13 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
+        <v>124</v>
+      </c>
+      <c r="I10" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10" t="s">
         <v>126</v>
-      </c>
-      <c r="I10" t="s">
-        <v>134</v>
-      </c>
-      <c r="J10" t="s">
-        <v>128</v>
       </c>
       <c r="K10" t="s">
         <v>25</v>
@@ -1923,25 +1941,25 @@
         <v>24</v>
       </c>
       <c r="N10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R10">
         <v>12</v>
       </c>
       <c r="S10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U10">
         <v>60</v>
@@ -1953,48 +1971,48 @@
         <v>41</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z10" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AB10" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC10" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD10" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE10">
         <v>4</v>
       </c>
       <c r="AF10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
@@ -2003,13 +2021,13 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" t="s">
+        <v>133</v>
+      </c>
+      <c r="J11" t="s">
         <v>126</v>
-      </c>
-      <c r="I11" t="s">
-        <v>135</v>
-      </c>
-      <c r="J11" t="s">
-        <v>128</v>
       </c>
       <c r="K11" t="s">
         <v>25</v>
@@ -2021,25 +2039,25 @@
         <v>24</v>
       </c>
       <c r="N11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P11">
         <v>1</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R11">
         <v>12</v>
       </c>
       <c r="S11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U11">
         <v>60</v>
@@ -2051,48 +2069,48 @@
         <v>41</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z11" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA11" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AB11" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC11" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD11" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE11">
         <v>4</v>
       </c>
       <c r="AF11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F12" s="3">
         <v>2</v>
@@ -2101,13 +2119,13 @@
         <v>2</v>
       </c>
       <c r="H12" t="s">
+        <v>124</v>
+      </c>
+      <c r="I12" t="s">
+        <v>134</v>
+      </c>
+      <c r="J12" t="s">
         <v>126</v>
-      </c>
-      <c r="I12" t="s">
-        <v>136</v>
-      </c>
-      <c r="J12" t="s">
-        <v>128</v>
       </c>
       <c r="K12" t="s">
         <v>25</v>
@@ -2122,22 +2140,22 @@
         <v>33</v>
       </c>
       <c r="O12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P12">
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R12">
         <v>12</v>
       </c>
       <c r="S12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U12">
         <v>60</v>
@@ -2149,22 +2167,22 @@
         <v>41</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z12" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA12" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AB12" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC12" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD12" t="s">
         <v>172</v>
@@ -2173,24 +2191,24 @@
         <v>4</v>
       </c>
       <c r="AF12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F13" s="3">
         <v>2</v>
@@ -2199,13 +2217,13 @@
         <v>2</v>
       </c>
       <c r="H13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" t="s">
+        <v>135</v>
+      </c>
+      <c r="J13" t="s">
         <v>126</v>
-      </c>
-      <c r="I13" t="s">
-        <v>137</v>
-      </c>
-      <c r="J13" t="s">
-        <v>128</v>
       </c>
       <c r="K13" t="s">
         <v>25</v>
@@ -2220,22 +2238,22 @@
         <v>33</v>
       </c>
       <c r="O13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P13">
         <v>1</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R13">
         <v>12</v>
       </c>
       <c r="S13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U13">
         <v>60</v>
@@ -2247,48 +2265,48 @@
         <v>41</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z13" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA13" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="AB13" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC13" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD13" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE13">
         <v>4</v>
       </c>
       <c r="AF13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F14" s="3">
         <v>2</v>
@@ -2297,13 +2315,13 @@
         <v>2</v>
       </c>
       <c r="H14" t="s">
+        <v>124</v>
+      </c>
+      <c r="I14" t="s">
+        <v>136</v>
+      </c>
+      <c r="J14" t="s">
         <v>126</v>
-      </c>
-      <c r="I14" t="s">
-        <v>138</v>
-      </c>
-      <c r="J14" t="s">
-        <v>128</v>
       </c>
       <c r="K14" t="s">
         <v>25</v>
@@ -2318,22 +2336,22 @@
         <v>33</v>
       </c>
       <c r="O14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P14">
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R14">
         <v>12</v>
       </c>
       <c r="S14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U14">
         <v>60</v>
@@ -2345,22 +2363,22 @@
         <v>41</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z14" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA14" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AB14" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC14" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD14" t="s">
         <v>172</v>
@@ -2369,24 +2387,24 @@
         <v>4</v>
       </c>
       <c r="AF14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F15" s="3">
         <v>2</v>
@@ -2395,13 +2413,13 @@
         <v>2</v>
       </c>
       <c r="H15" t="s">
+        <v>124</v>
+      </c>
+      <c r="I15" t="s">
+        <v>148</v>
+      </c>
+      <c r="J15" t="s">
         <v>126</v>
-      </c>
-      <c r="I15" t="s">
-        <v>150</v>
-      </c>
-      <c r="J15" t="s">
-        <v>128</v>
       </c>
       <c r="K15" t="s">
         <v>25</v>
@@ -2413,25 +2431,25 @@
         <v>24</v>
       </c>
       <c r="N15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R15">
         <v>12</v>
       </c>
       <c r="S15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U15">
         <v>60</v>
@@ -2443,48 +2461,48 @@
         <v>41</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z15" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA15" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AB15" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC15" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD15" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE15">
         <v>4</v>
       </c>
       <c r="AF15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F16" s="3">
         <v>2</v>
@@ -2493,13 +2511,13 @@
         <v>2</v>
       </c>
       <c r="H16" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" t="s">
+        <v>149</v>
+      </c>
+      <c r="J16" t="s">
         <v>126</v>
-      </c>
-      <c r="I16" t="s">
-        <v>151</v>
-      </c>
-      <c r="J16" t="s">
-        <v>128</v>
       </c>
       <c r="K16" t="s">
         <v>25</v>
@@ -2511,25 +2529,25 @@
         <v>24</v>
       </c>
       <c r="N16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P16">
         <v>1</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R16">
         <v>12</v>
       </c>
       <c r="S16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U16">
         <v>60</v>
@@ -2541,48 +2559,48 @@
         <v>41</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z16" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA16" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AB16" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC16" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD16" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE16">
         <v>4</v>
       </c>
       <c r="AF16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F17" s="3">
         <v>2</v>
@@ -2591,13 +2609,13 @@
         <v>2</v>
       </c>
       <c r="H17" t="s">
+        <v>124</v>
+      </c>
+      <c r="I17" t="s">
+        <v>150</v>
+      </c>
+      <c r="J17" t="s">
         <v>126</v>
-      </c>
-      <c r="I17" t="s">
-        <v>152</v>
-      </c>
-      <c r="J17" t="s">
-        <v>128</v>
       </c>
       <c r="K17" t="s">
         <v>25</v>
@@ -2609,25 +2627,25 @@
         <v>24</v>
       </c>
       <c r="N17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P17">
         <v>0</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R17">
         <v>12</v>
       </c>
       <c r="S17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U17">
         <v>60</v>
@@ -2639,48 +2657,48 @@
         <v>41</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z17" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA17" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AB17" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC17" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD17" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE17">
         <v>4</v>
       </c>
       <c r="AF17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F18" s="3">
         <v>2</v>
@@ -2689,13 +2707,13 @@
         <v>2</v>
       </c>
       <c r="H18" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" t="s">
+        <v>151</v>
+      </c>
+      <c r="J18" t="s">
         <v>126</v>
-      </c>
-      <c r="I18" t="s">
-        <v>153</v>
-      </c>
-      <c r="J18" t="s">
-        <v>128</v>
       </c>
       <c r="K18" t="s">
         <v>25</v>
@@ -2707,25 +2725,25 @@
         <v>24</v>
       </c>
       <c r="N18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P18">
         <v>0</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R18">
         <v>12</v>
       </c>
       <c r="S18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U18">
         <v>60</v>
@@ -2737,22 +2755,22 @@
         <v>41</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z18" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA18" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AB18" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC18" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD18" t="s">
         <v>172</v>
@@ -2761,24 +2779,24 @@
         <v>4</v>
       </c>
       <c r="AF18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19" s="3">
         <v>0</v>
@@ -2787,13 +2805,13 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" t="s">
+        <v>152</v>
+      </c>
+      <c r="J19" t="s">
         <v>126</v>
-      </c>
-      <c r="I19" t="s">
-        <v>154</v>
-      </c>
-      <c r="J19" t="s">
-        <v>128</v>
       </c>
       <c r="K19" t="s">
         <v>25</v>
@@ -2805,25 +2823,25 @@
         <v>24</v>
       </c>
       <c r="N19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P19">
         <v>1</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R19">
         <v>12</v>
       </c>
       <c r="S19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U19">
         <v>60</v>
@@ -2835,48 +2853,48 @@
         <v>41</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z19" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA19" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AB19" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC19" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD19" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE19">
         <v>4</v>
       </c>
       <c r="AF19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F20" s="3">
         <v>0</v>
@@ -2885,13 +2903,13 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
+        <v>124</v>
+      </c>
+      <c r="I20" t="s">
+        <v>153</v>
+      </c>
+      <c r="J20" t="s">
         <v>126</v>
-      </c>
-      <c r="I20" t="s">
-        <v>155</v>
-      </c>
-      <c r="J20" t="s">
-        <v>128</v>
       </c>
       <c r="K20" t="s">
         <v>25</v>
@@ -2903,25 +2921,25 @@
         <v>24</v>
       </c>
       <c r="N20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P20">
         <v>0</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R20">
         <v>12</v>
       </c>
       <c r="S20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U20">
         <v>60</v>
@@ -2933,22 +2951,22 @@
         <v>41</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z20" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA20" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AB20" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC20" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD20" t="s">
         <v>172</v>
@@ -2957,24 +2975,24 @@
         <v>4</v>
       </c>
       <c r="AF20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F21" s="3">
         <v>0</v>
@@ -2983,13 +3001,13 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
+        <v>124</v>
+      </c>
+      <c r="I21" t="s">
+        <v>154</v>
+      </c>
+      <c r="J21" t="s">
         <v>126</v>
-      </c>
-      <c r="I21" t="s">
-        <v>156</v>
-      </c>
-      <c r="J21" t="s">
-        <v>128</v>
       </c>
       <c r="K21" t="s">
         <v>25</v>
@@ -3001,25 +3019,25 @@
         <v>24</v>
       </c>
       <c r="N21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P21">
         <v>1</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R21">
         <v>12</v>
       </c>
       <c r="S21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U21">
         <v>60</v>
@@ -3031,22 +3049,22 @@
         <v>41</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z21" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA21" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AB21" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC21" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD21" t="s">
         <v>172</v>
@@ -3055,24 +3073,24 @@
         <v>4</v>
       </c>
       <c r="AF21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F22" s="3">
         <v>0</v>
@@ -3081,13 +3099,13 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
+        <v>124</v>
+      </c>
+      <c r="I22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J22" t="s">
         <v>126</v>
-      </c>
-      <c r="I22" t="s">
-        <v>157</v>
-      </c>
-      <c r="J22" t="s">
-        <v>128</v>
       </c>
       <c r="K22" t="s">
         <v>25</v>
@@ -3099,25 +3117,25 @@
         <v>24</v>
       </c>
       <c r="N22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P22">
         <v>1</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R22">
         <v>12</v>
       </c>
       <c r="S22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U22">
         <v>60</v>
@@ -3129,48 +3147,48 @@
         <v>41</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z22" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA22" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AB22" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC22" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD22" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE22">
         <v>4</v>
       </c>
       <c r="AF22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F23" s="3">
         <v>0</v>
@@ -3179,13 +3197,13 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
+        <v>124</v>
+      </c>
+      <c r="I23" t="s">
+        <v>156</v>
+      </c>
+      <c r="J23" t="s">
         <v>126</v>
-      </c>
-      <c r="I23" t="s">
-        <v>158</v>
-      </c>
-      <c r="J23" t="s">
-        <v>128</v>
       </c>
       <c r="K23" t="s">
         <v>25</v>
@@ -3197,25 +3215,25 @@
         <v>24</v>
       </c>
       <c r="N23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P23">
         <v>1</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R23">
         <v>12</v>
       </c>
       <c r="S23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U23">
         <v>60</v>
@@ -3227,22 +3245,22 @@
         <v>41</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y23" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z23" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA23" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AB23" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC23" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD23" t="s">
         <v>172</v>
@@ -3251,24 +3269,24 @@
         <v>4</v>
       </c>
       <c r="AF23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F24" s="3">
         <v>0</v>
@@ -3277,13 +3295,13 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
+        <v>124</v>
+      </c>
+      <c r="I24" t="s">
+        <v>157</v>
+      </c>
+      <c r="J24" t="s">
         <v>126</v>
-      </c>
-      <c r="I24" t="s">
-        <v>159</v>
-      </c>
-      <c r="J24" t="s">
-        <v>128</v>
       </c>
       <c r="K24" t="s">
         <v>25</v>
@@ -3295,25 +3313,25 @@
         <v>24</v>
       </c>
       <c r="N24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P24">
         <v>0</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R24">
         <v>12</v>
       </c>
       <c r="S24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U24">
         <v>60</v>
@@ -3325,48 +3343,48 @@
         <v>41</v>
       </c>
       <c r="X24" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y24" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z24" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA24" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AB24" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC24" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD24" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE24">
         <v>4</v>
       </c>
       <c r="AF24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F25" s="3">
         <v>0</v>
@@ -3375,13 +3393,13 @@
         <v>0</v>
       </c>
       <c r="H25" t="s">
+        <v>124</v>
+      </c>
+      <c r="I25" t="s">
+        <v>158</v>
+      </c>
+      <c r="J25" t="s">
         <v>126</v>
-      </c>
-      <c r="I25" t="s">
-        <v>160</v>
-      </c>
-      <c r="J25" t="s">
-        <v>128</v>
       </c>
       <c r="K25" t="s">
         <v>25</v>
@@ -3393,25 +3411,25 @@
         <v>24</v>
       </c>
       <c r="N25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P25">
         <v>0</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R25">
         <v>12</v>
       </c>
       <c r="S25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U25">
         <v>60</v>
@@ -3423,48 +3441,48 @@
         <v>41</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y25" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z25" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA25" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AB25" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC25" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD25" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE25">
         <v>4</v>
       </c>
       <c r="AF25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F26" s="3">
         <v>0</v>
@@ -3473,13 +3491,13 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
+        <v>124</v>
+      </c>
+      <c r="I26" t="s">
+        <v>159</v>
+      </c>
+      <c r="J26" t="s">
         <v>126</v>
-      </c>
-      <c r="I26" t="s">
-        <v>161</v>
-      </c>
-      <c r="J26" t="s">
-        <v>128</v>
       </c>
       <c r="K26" t="s">
         <v>25</v>
@@ -3491,25 +3509,25 @@
         <v>24</v>
       </c>
       <c r="N26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P26">
         <v>0</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R26">
         <v>12</v>
       </c>
       <c r="S26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U26">
         <v>60</v>
@@ -3521,34 +3539,34 @@
         <v>41</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z26" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA26" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AB26" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC26" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD26" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE26">
         <v>4</v>
       </c>
       <c r="AF26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -3559,10 +3577,10 @@
         <v>27</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F27" s="3">
         <v>2</v>
@@ -3571,13 +3589,13 @@
         <v>2</v>
       </c>
       <c r="H27" t="s">
+        <v>124</v>
+      </c>
+      <c r="I27" t="s">
+        <v>170</v>
+      </c>
+      <c r="J27" t="s">
         <v>126</v>
-      </c>
-      <c r="I27" t="s">
-        <v>173</v>
-      </c>
-      <c r="J27" t="s">
-        <v>128</v>
       </c>
       <c r="K27" t="s">
         <v>25</v>
@@ -3589,25 +3607,25 @@
         <v>24</v>
       </c>
       <c r="N27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P27">
         <v>0</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R27">
         <v>12</v>
       </c>
       <c r="S27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U27">
         <v>60</v>
@@ -3619,39 +3637,48 @@
         <v>41</v>
       </c>
       <c r="X27" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Y27" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z27" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AA27" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AB27" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC27" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD27" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="AE27">
         <v>4</v>
       </c>
       <c r="AF27" t="s">
+        <v>171</v>
+      </c>
+      <c r="AH27" t="s">
         <v>175</v>
       </c>
+      <c r="AI27" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>27</v>
@@ -3717,14 +3744,14 @@
         <v>43</v>
       </c>
       <c r="Y28" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
       <c r="AD28" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="AE28">
         <v>1</v>
@@ -3733,12 +3760,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>27</v>
@@ -3804,14 +3831,14 @@
         <v>43</v>
       </c>
       <c r="Y29" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z29" s="5"/>
       <c r="AA29" s="5"/>
       <c r="AB29" s="5"/>
       <c r="AC29" s="5"/>
       <c r="AD29" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="AE29">
         <v>1</v>
@@ -3820,12 +3847,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>27</v>
@@ -3898,7 +3925,7 @@
       <c r="AB30" s="5"/>
       <c r="AC30" s="5"/>
       <c r="AD30" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="AE30">
         <v>1</v>
@@ -3907,12 +3934,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>27</v>
@@ -3985,7 +4012,7 @@
       <c r="AB31" s="5"/>
       <c r="AC31" s="5"/>
       <c r="AD31" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="AE31">
         <v>1</v>
@@ -3994,12 +4021,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>27</v>
@@ -4072,7 +4099,7 @@
       <c r="AB32" s="5"/>
       <c r="AC32" s="5"/>
       <c r="AD32" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="AE32">
         <v>1</v>
@@ -4086,7 +4113,7 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>27</v>
@@ -4159,7 +4186,7 @@
       <c r="AB33" s="5"/>
       <c r="AC33" s="5"/>
       <c r="AD33" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="AE33">
         <v>1</v>
@@ -4173,7 +4200,7 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>27</v>
@@ -4246,7 +4273,7 @@
       <c r="AB34" s="5"/>
       <c r="AC34" s="5"/>
       <c r="AD34" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="AE34">
         <v>1</v>
@@ -4260,7 +4287,7 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>27</v>
@@ -4333,7 +4360,7 @@
       <c r="AB35" s="5"/>
       <c r="AC35" s="5"/>
       <c r="AD35" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="AE35">
         <v>1</v>
@@ -4347,7 +4374,7 @@
         <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>27</v>
@@ -4420,7 +4447,7 @@
       <c r="AB36" s="5"/>
       <c r="AC36" s="5"/>
       <c r="AD36" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="AE36">
         <v>1</v>
@@ -4434,7 +4461,7 @@
         <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>27</v>
@@ -4507,7 +4534,7 @@
       <c r="AB37" s="5"/>
       <c r="AC37" s="5"/>
       <c r="AD37" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="AE37">
         <v>1</v>

</xml_diff>